<commit_message>
add a new feature validation and auth
</commit_message>
<xml_diff>
--- a/blanco-meta/rest/CheckTokenApi.xlsx
+++ b/blanco-meta/rest/CheckTokenApi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuji/projects/dapanda/assemulator/blanco-meta/rest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuji/projects/dapanda/dapanda-api-core/blanco-meta/rest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3297699-525F-184E-A5CC-47BB13F57551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B046EB-D157-9441-A167-4195731160B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="1220" windowWidth="24600" windowHeight="14720" tabRatio="641" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2560" yWindow="1480" windowWidth="24600" windowHeight="14720" tabRatio="641" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="190">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2208,6 +2208,9 @@
   <si>
     <t>dapanda.api.common</t>
     <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -3920,6 +3923,9 @@
             <v>query</v>
           </cell>
         </row>
+        <row r="7">
+          <cell r="G7"/>
+        </row>
       </sheetData>
     </sheetDataSet>
   </externalBook>
@@ -4266,8 +4272,8 @@
   </sheetPr>
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:E10"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4458,7 +4464,9 @@
       </c>
       <c r="B16" s="201"/>
       <c r="C16" s="202"/>
-      <c r="D16" s="103"/>
+      <c r="D16" s="103" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="204" t="s">
@@ -7045,7 +7053,7 @@
   </sheetPr>
   <dimension ref="A1:T61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix rest api object
</commit_message>
<xml_diff>
--- a/blanco-meta/rest/CheckTokenApi.xlsx
+++ b/blanco-meta/rest/CheckTokenApi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuji/projects/dapanda/dapanda-api-core/blanco-meta/rest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B046EB-D157-9441-A167-4195731160B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04EE24E-66DC-2F47-A48A-E3560168F10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2560" yWindow="1480" windowWidth="24600" windowHeight="14720" tabRatio="641" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="191">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -2211,6 +2211,10 @@
   </si>
   <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>blanco.restgenerator.valueobject.ResponseHeader</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -4272,8 +4276,8 @@
   </sheetPr>
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4455,7 +4459,9 @@
       </c>
       <c r="B15" s="197"/>
       <c r="C15" s="197"/>
-      <c r="D15" s="198"/>
+      <c r="D15" s="198" t="s">
+        <v>190</v>
+      </c>
       <c r="E15" s="199"/>
     </row>
     <row r="16" spans="1:8">
@@ -5238,7 +5244,7 @@
   <dimension ref="A1:AB104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+      <selection activeCell="C16" sqref="C16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>

</xml_diff>